<commit_message>
Added index, signup, signin and semi-main page. Inf loop bug
</commit_message>
<xml_diff>
--- a/Relacion de Tablas de BD.xlsx
+++ b/Relacion de Tablas de BD.xlsx
@@ -69,9 +69,6 @@
     <t>img_content</t>
   </si>
   <si>
-    <t>date_sent</t>
-  </si>
-  <si>
     <t>online</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>administrator</t>
+  </si>
+  <si>
+    <t>sent_at</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,15 +521,15 @@
         <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="23.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -554,12 +554,12 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="23.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -572,12 +572,12 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="23.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -590,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>